<commit_message>
Zeitplan update & Dokumentation Planen abgeschlossen
</commit_message>
<xml_diff>
--- a/Documents/Gantt.xlsx
+++ b/Documents/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsordner\_ImportantStuff\IPA\Probe\MyMuesli\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94E24F33-E4E1-4146-AF97-7B60A8B03900}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D80BF98D-4AEF-4A48-85B4-E7369571E8A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{7368EEC8-37A3-4D19-88FF-F7E147FC3DC2}"/>
   </bookViews>
@@ -235,7 +235,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +278,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -814,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1022,33 +1028,93 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1061,65 +1127,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1437,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D6F5E9-624B-4CCE-882E-0793EA18CA51}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,62 +1471,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="100"/>
+      <c r="C1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="72" t="s">
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="72" t="s">
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="72" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="72" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="74"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="98"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="77"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="99"/>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="39" t="s">
         <v>2</v>
       </c>
@@ -1553,10 +1577,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="95" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -1578,12 +1602,12 @@
       <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="93"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="104"/>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
       <c r="G5" s="14"/>
@@ -1600,8 +1624,8 @@
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="94"/>
-      <c r="B6" s="71" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1624,13 +1648,13 @@
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="94"/>
-      <c r="B7" s="71"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
+      <c r="E7" s="105"/>
       <c r="F7" s="29"/>
       <c r="G7" s="14"/>
       <c r="H7" s="13"/>
@@ -1646,8 +1670,8 @@
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="94"/>
-      <c r="B8" s="71" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="96" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -1670,14 +1694,14 @@
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="94"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="14"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -1692,8 +1716,8 @@
       <c r="R9" s="15"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="94"/>
-      <c r="B10" s="71" t="s">
+      <c r="A10" s="93"/>
+      <c r="B10" s="96" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1716,14 +1740,14 @@
       <c r="R10" s="15"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="94"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="14"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -1738,10 +1762,10 @@
       <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="95" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="23" t="s">
@@ -1764,15 +1788,15 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="94"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="43" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="106"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="12"/>
@@ -1786,8 +1810,8 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="94"/>
-      <c r="B14" s="71" t="s">
+      <c r="A14" s="93"/>
+      <c r="B14" s="96" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -1810,8 +1834,8 @@
       <c r="R14" s="13"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="94"/>
-      <c r="B15" s="71"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="42" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1843,7 @@
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="31"/>
-      <c r="H15" s="29"/>
+      <c r="H15" s="105"/>
       <c r="I15" s="29"/>
       <c r="J15" s="12"/>
       <c r="K15" s="13"/>
@@ -1832,8 +1856,8 @@
       <c r="R15" s="13"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="94"/>
-      <c r="B16" s="71" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="96" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="22" t="s">
@@ -1856,8 +1880,8 @@
       <c r="R16" s="13"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="94"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="42" t="s">
         <v>6</v>
       </c>
@@ -1866,7 +1890,7 @@
       <c r="F17" s="29"/>
       <c r="G17" s="31"/>
       <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="12"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -1878,8 +1902,8 @@
       <c r="R17" s="13"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="94"/>
-      <c r="B18" s="79" t="s">
+      <c r="A18" s="93"/>
+      <c r="B18" s="75" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="56" t="s">
@@ -1902,8 +1926,8 @@
       <c r="R18" s="13"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="94"/>
-      <c r="B19" s="90"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="42" t="s">
         <v>6</v>
       </c>
@@ -1911,8 +1935,8 @@
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="31"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
       <c r="J19" s="12"/>
       <c r="K19" s="13"/>
       <c r="L19" s="29"/>
@@ -1924,8 +1948,8 @@
       <c r="R19" s="13"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="94"/>
-      <c r="B20" s="71" t="s">
+      <c r="A20" s="93"/>
+      <c r="B20" s="96" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="22" t="s">
@@ -1948,8 +1972,8 @@
       <c r="R20" s="13"/>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="95"/>
-      <c r="B21" s="96"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="44" t="s">
         <v>6</v>
       </c>
@@ -1958,7 +1982,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="32"/>
       <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="32"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -1970,10 +1994,10 @@
       <c r="R21" s="17"/>
     </row>
     <row r="22" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="75" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="25" t="s">
@@ -1996,8 +2020,8 @@
       <c r="R22" s="19"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
-      <c r="B23" s="90"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="45" t="s">
         <v>6</v>
       </c>
@@ -2018,8 +2042,8 @@
       <c r="R23" s="19"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="89"/>
-      <c r="B24" s="79" t="s">
+      <c r="A24" s="78"/>
+      <c r="B24" s="75" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -2042,8 +2066,8 @@
       <c r="R24" s="19"/>
     </row>
     <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="89"/>
-      <c r="B25" s="90"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="43" t="s">
         <v>6</v>
       </c>
@@ -2064,10 +2088,10 @@
       <c r="R25" s="19"/>
     </row>
     <row r="26" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="90" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="21" t="s">
@@ -2089,8 +2113,8 @@
       <c r="R26" s="11"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="90"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="46" t="s">
         <v>6</v>
       </c>
@@ -2111,8 +2135,8 @@
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="79" t="s">
+      <c r="A28" s="78"/>
+      <c r="B28" s="75" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -2134,8 +2158,8 @@
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="90"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="46" t="s">
         <v>6</v>
       </c>
@@ -2156,8 +2180,8 @@
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="89"/>
-      <c r="B30" s="79" t="s">
+      <c r="A30" s="78"/>
+      <c r="B30" s="75" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="26" t="s">
@@ -2180,8 +2204,8 @@
       <c r="R30" s="13"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="89"/>
-      <c r="B31" s="90"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="46" t="s">
         <v>6</v>
       </c>
@@ -2202,8 +2226,8 @@
       <c r="R31" s="13"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
-      <c r="B32" s="79" t="s">
+      <c r="A32" s="78"/>
+      <c r="B32" s="75" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="24" t="s">
@@ -2226,8 +2250,8 @@
       <c r="R32" s="13"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="89"/>
-      <c r="B33" s="87"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="43" t="s">
         <v>6</v>
       </c>
@@ -2248,8 +2272,8 @@
       <c r="R33" s="29"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="89"/>
-      <c r="B34" s="79" t="s">
+      <c r="A34" s="78"/>
+      <c r="B34" s="75" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="25" t="s">
@@ -2272,8 +2296,8 @@
       <c r="R34" s="29"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="89"/>
-      <c r="B35" s="90"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="76"/>
       <c r="C35" s="42" t="s">
         <v>6</v>
       </c>
@@ -2294,8 +2318,8 @@
       <c r="R35" s="29"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="89"/>
-      <c r="B36" s="79" t="s">
+      <c r="A36" s="78"/>
+      <c r="B36" s="75" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="22" t="s">
@@ -2318,8 +2342,8 @@
       <c r="R36" s="29"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="89"/>
-      <c r="B37" s="90"/>
+      <c r="A37" s="78"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="43" t="s">
         <v>6</v>
       </c>
@@ -2340,8 +2364,8 @@
       <c r="R37" s="29"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="89"/>
-      <c r="B38" s="79" t="s">
+      <c r="A38" s="78"/>
+      <c r="B38" s="75" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="22" t="s">
@@ -2364,8 +2388,8 @@
       <c r="R38" s="29"/>
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="89"/>
-      <c r="B39" s="90"/>
+      <c r="A39" s="78"/>
+      <c r="B39" s="76"/>
       <c r="C39" s="43" t="s">
         <v>6</v>
       </c>
@@ -2386,10 +2410,10 @@
       <c r="R39" s="29"/>
     </row>
     <row r="40" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="88" t="s">
+      <c r="A40" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="86" t="s">
+      <c r="B40" s="90" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="21" t="s">
@@ -2412,8 +2436,8 @@
       <c r="R40" s="11"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="89"/>
-      <c r="B41" s="90"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="42" t="s">
         <v>6</v>
       </c>
@@ -2434,8 +2458,8 @@
       <c r="R41" s="13"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="89"/>
-      <c r="B42" s="79" t="s">
+      <c r="A42" s="78"/>
+      <c r="B42" s="75" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="22" t="s">
@@ -2458,8 +2482,8 @@
       <c r="R42" s="13"/>
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="91"/>
-      <c r="B43" s="92"/>
+      <c r="A43" s="82"/>
+      <c r="B43" s="91"/>
       <c r="C43" s="44" t="s">
         <v>6</v>
       </c>
@@ -2480,10 +2504,10 @@
       <c r="R43" s="17"/>
     </row>
     <row r="44" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="86" t="s">
+      <c r="B44" s="90" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="21" t="s">
@@ -2506,8 +2530,8 @@
       <c r="R44" s="11"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="89"/>
-      <c r="B45" s="87"/>
+      <c r="A45" s="78"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="46" t="s">
         <v>6</v>
       </c>
@@ -2528,8 +2552,8 @@
       <c r="R45" s="13"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="89"/>
-      <c r="B46" s="79" t="s">
+      <c r="A46" s="78"/>
+      <c r="B46" s="75" t="s">
         <v>43</v>
       </c>
       <c r="C46" s="24" t="s">
@@ -2552,8 +2576,8 @@
       <c r="R46" s="29"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="89"/>
-      <c r="B47" s="90"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="43" t="s">
         <v>6</v>
       </c>
@@ -2574,8 +2598,8 @@
       <c r="R47" s="29"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="89"/>
-      <c r="B48" s="79" t="s">
+      <c r="A48" s="78"/>
+      <c r="B48" s="75" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -2598,8 +2622,8 @@
       <c r="R48" s="60"/>
     </row>
     <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="97"/>
-      <c r="B49" s="98"/>
+      <c r="A49" s="79"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="53" t="s">
         <v>6</v>
       </c>
@@ -2620,8 +2644,8 @@
       <c r="R49" s="48"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="89"/>
-      <c r="B50" s="99" t="s">
+      <c r="A50" s="78"/>
+      <c r="B50" s="83" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="52" t="s">
@@ -2644,12 +2668,12 @@
       <c r="R50" s="51"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="89"/>
-      <c r="B51" s="90"/>
+      <c r="A51" s="78"/>
+      <c r="B51" s="76"/>
       <c r="C51" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="31"/>
+      <c r="D51" s="106"/>
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
       <c r="G51" s="31"/>
@@ -2666,8 +2690,8 @@
       <c r="R51" s="29"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="89"/>
-      <c r="B52" s="87" t="s">
+      <c r="A52" s="78"/>
+      <c r="B52" s="80" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="54" t="s">
@@ -2690,17 +2714,17 @@
       <c r="R52" s="57"/>
     </row>
     <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="91"/>
-      <c r="B53" s="90"/>
+      <c r="A53" s="82"/>
+      <c r="B53" s="76"/>
       <c r="C53" s="43" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="47"/>
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
-      <c r="G53" s="47"/>
+      <c r="G53" s="107"/>
       <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
+      <c r="I53" s="108"/>
       <c r="J53" s="47"/>
       <c r="K53" s="48"/>
       <c r="L53" s="48"/>
@@ -2749,6 +2773,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="M1:O2"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A26:A39"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="J1:L2"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="B38:B39"/>
@@ -2765,30 +2813,6 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="M1:O2"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A26:A39"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A12:A21"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="J1:L2"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="G1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2806,117 +2830,117 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100">
+      <c r="A1" s="71">
         <v>0.75</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="101">
+      <c r="A2" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="102">
+      <c r="A3" s="73">
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="101">
+      <c r="A4" s="72">
         <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="102">
+      <c r="A5" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="101">
+      <c r="A6" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="102">
+      <c r="A7" s="73">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="101">
+      <c r="A8" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="102">
+      <c r="A9" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="101">
+      <c r="A10" s="72">
         <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="102">
+      <c r="A11" s="73">
         <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="101">
+      <c r="A12" s="72">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="102">
+      <c r="A13" s="73">
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="101">
+      <c r="A14" s="72">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="102">
+      <c r="A15" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="101">
+      <c r="A16" s="72">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="102">
+      <c r="A17" s="73">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="101">
+      <c r="A18" s="72">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="102">
+      <c r="A19" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="101">
+      <c r="A20" s="72">
         <v>1.25</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="102">
+      <c r="A21" s="73">
         <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="101">
+      <c r="A22" s="72">
         <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="103">
+      <c r="A23" s="74">
         <v>1.5</v>
       </c>
       <c r="D23">

</xml_diff>

<commit_message>
UnitTests eingecheckt &  letzte View  & ViewModel änderungen
</commit_message>
<xml_diff>
--- a/Documents/Gantt.xlsx
+++ b/Documents/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsordner\_ImportantStuff\IPA\Probe\MyMuesli\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F74091B9-8783-40AC-8D6F-7972A941B3F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1FBD9464-3033-4D12-BE55-82BF7052535F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{7368EEC8-37A3-4D19-88FF-F7E147FC3DC2}"/>
   </bookViews>
@@ -1061,92 +1061,92 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D6F5E9-624B-4CCE-882E-0793EA18CA51}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,62 +1474,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="109" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="93" t="s">
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="93" t="s">
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="93" t="s">
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="93" t="s">
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="105"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="85"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="106"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="88"/>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="108"/>
-      <c r="B3" s="108"/>
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="39" t="s">
         <v>2</v>
       </c>
@@ -1580,10 +1580,10 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="89" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -1605,8 +1605,8 @@
       <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
-      <c r="B5" s="82"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="42" t="s">
         <v>6</v>
       </c>
@@ -1627,8 +1627,8 @@
       <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
-      <c r="B6" s="103" t="s">
+      <c r="A6" s="105"/>
+      <c r="B6" s="82" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1651,8 +1651,8 @@
       <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="42" t="s">
         <v>6</v>
       </c>
@@ -1673,8 +1673,8 @@
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
-      <c r="B8" s="103" t="s">
+      <c r="A8" s="105"/>
+      <c r="B8" s="82" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="22" t="s">
@@ -1697,8 +1697,8 @@
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="100"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="42" t="s">
         <v>6</v>
       </c>
@@ -1719,8 +1719,8 @@
       <c r="R9" s="15"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="103" t="s">
+      <c r="A10" s="105"/>
+      <c r="B10" s="82" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -1743,8 +1743,8 @@
       <c r="R10" s="15"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="100"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="42" t="s">
         <v>6</v>
       </c>
@@ -1765,10 +1765,10 @@
       <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="89" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="23" t="s">
@@ -1791,8 +1791,8 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
-      <c r="B13" s="103"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="43" t="s">
         <v>6</v>
       </c>
@@ -1813,8 +1813,8 @@
       <c r="R13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="103" t="s">
+      <c r="A14" s="105"/>
+      <c r="B14" s="82" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -1837,8 +1837,8 @@
       <c r="R14" s="13"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="105"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="42" t="s">
         <v>6</v>
       </c>
@@ -1859,8 +1859,8 @@
       <c r="R15" s="13"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="105"/>
+      <c r="B16" s="82" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="22" t="s">
@@ -1883,8 +1883,8 @@
       <c r="R16" s="13"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="103"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="42" t="s">
         <v>6</v>
       </c>
@@ -1905,8 +1905,8 @@
       <c r="R17" s="13"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="82" t="s">
+      <c r="A18" s="105"/>
+      <c r="B18" s="90" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="56" t="s">
@@ -1929,8 +1929,8 @@
       <c r="R18" s="13"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="105"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="42" t="s">
         <v>6</v>
       </c>
@@ -1951,8 +1951,8 @@
       <c r="R19" s="13"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
-      <c r="B20" s="103" t="s">
+      <c r="A20" s="105"/>
+      <c r="B20" s="82" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="22" t="s">
@@ -1975,8 +1975,8 @@
       <c r="R20" s="13"/>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="101"/>
-      <c r="B21" s="104"/>
+      <c r="A21" s="106"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="44" t="s">
         <v>6</v>
       </c>
@@ -1997,10 +1997,10 @@
       <c r="R21" s="17"/>
     </row>
     <row r="22" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="90" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="25" t="s">
@@ -2023,8 +2023,8 @@
       <c r="R22" s="19"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="85"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="101"/>
       <c r="C23" s="45" t="s">
         <v>6</v>
       </c>
@@ -2045,8 +2045,8 @@
       <c r="R23" s="19"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="85"/>
-      <c r="B24" s="82" t="s">
+      <c r="A24" s="100"/>
+      <c r="B24" s="90" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -2069,8 +2069,8 @@
       <c r="R24" s="19"/>
     </row>
     <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="85"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="101"/>
       <c r="C25" s="43" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="R25" s="19"/>
     </row>
     <row r="26" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="84" t="s">
+      <c r="A26" s="99" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="97" t="s">
@@ -2116,8 +2116,8 @@
       <c r="R26" s="11"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="85"/>
-      <c r="B27" s="83"/>
+      <c r="A27" s="100"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="46" t="s">
         <v>6</v>
       </c>
@@ -2138,8 +2138,8 @@
       <c r="R27" s="13"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="82" t="s">
+      <c r="A28" s="100"/>
+      <c r="B28" s="90" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -2161,8 +2161,8 @@
       <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="85"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="100"/>
+      <c r="B29" s="101"/>
       <c r="C29" s="46" t="s">
         <v>6</v>
       </c>
@@ -2183,8 +2183,8 @@
       <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
-      <c r="B30" s="82" t="s">
+      <c r="A30" s="100"/>
+      <c r="B30" s="90" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="26" t="s">
@@ -2207,8 +2207,8 @@
       <c r="R30" s="13"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="85"/>
-      <c r="B31" s="83"/>
+      <c r="A31" s="100"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="46" t="s">
         <v>6</v>
       </c>
@@ -2229,8 +2229,8 @@
       <c r="R31" s="13"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="85"/>
-      <c r="B32" s="82" t="s">
+      <c r="A32" s="100"/>
+      <c r="B32" s="90" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="24" t="s">
@@ -2253,8 +2253,8 @@
       <c r="R32" s="13"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="85"/>
-      <c r="B33" s="87"/>
+      <c r="A33" s="100"/>
+      <c r="B33" s="98"/>
       <c r="C33" s="43" t="s">
         <v>6</v>
       </c>
@@ -2275,8 +2275,8 @@
       <c r="R33" s="29"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="85"/>
-      <c r="B34" s="82" t="s">
+      <c r="A34" s="100"/>
+      <c r="B34" s="90" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="25" t="s">
@@ -2299,8 +2299,8 @@
       <c r="R34" s="29"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="85"/>
-      <c r="B35" s="83"/>
+      <c r="A35" s="100"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="42" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="J35" s="31"/>
       <c r="K35" s="76"/>
       <c r="L35" s="76"/>
-      <c r="M35" s="31"/>
+      <c r="M35" s="77"/>
       <c r="N35" s="29"/>
       <c r="O35" s="29"/>
       <c r="P35" s="31"/>
@@ -2321,8 +2321,8 @@
       <c r="R35" s="29"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="85"/>
-      <c r="B36" s="82" t="s">
+      <c r="A36" s="100"/>
+      <c r="B36" s="90" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="22" t="s">
@@ -2345,8 +2345,8 @@
       <c r="R36" s="29"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="85"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="100"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="43" t="s">
         <v>6</v>
       </c>
@@ -2367,8 +2367,8 @@
       <c r="R37" s="29"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="85"/>
-      <c r="B38" s="82" t="s">
+      <c r="A38" s="100"/>
+      <c r="B38" s="90" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="22" t="s">
@@ -2391,8 +2391,8 @@
       <c r="R38" s="29"/>
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="85"/>
-      <c r="B39" s="83"/>
+      <c r="A39" s="100"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="43" t="s">
         <v>6</v>
       </c>
@@ -2405,15 +2405,15 @@
       <c r="J39" s="12"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="76"/>
+      <c r="O39" s="76"/>
       <c r="P39" s="31"/>
       <c r="Q39" s="29"/>
       <c r="R39" s="29"/>
     </row>
     <row r="40" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="99" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="97" t="s">
@@ -2439,8 +2439,8 @@
       <c r="R40" s="11"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="85"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="100"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="42" t="s">
         <v>6</v>
       </c>
@@ -2455,14 +2455,14 @@
       <c r="L41" s="13"/>
       <c r="M41" s="12"/>
       <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
+      <c r="O41" s="76"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="85"/>
-      <c r="B42" s="82" t="s">
+      <c r="A42" s="100"/>
+      <c r="B42" s="90" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="22" t="s">
@@ -2485,8 +2485,8 @@
       <c r="R42" s="13"/>
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="89"/>
-      <c r="B43" s="98"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="103"/>
       <c r="C43" s="44" t="s">
         <v>6</v>
       </c>
@@ -2501,13 +2501,13 @@
       <c r="L43" s="17"/>
       <c r="M43" s="18"/>
       <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="18"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="32"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="17"/>
     </row>
     <row r="44" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="84" t="s">
+      <c r="A44" s="99" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="97" t="s">
@@ -2533,8 +2533,8 @@
       <c r="R44" s="11"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="85"/>
-      <c r="B45" s="87"/>
+      <c r="A45" s="100"/>
+      <c r="B45" s="98"/>
       <c r="C45" s="46" t="s">
         <v>6</v>
       </c>
@@ -2555,8 +2555,8 @@
       <c r="R45" s="13"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="85"/>
-      <c r="B46" s="82" t="s">
+      <c r="A46" s="100"/>
+      <c r="B46" s="90" t="s">
         <v>43</v>
       </c>
       <c r="C46" s="24" t="s">
@@ -2579,8 +2579,8 @@
       <c r="R46" s="29"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="85"/>
-      <c r="B47" s="83"/>
+      <c r="A47" s="100"/>
+      <c r="B47" s="101"/>
       <c r="C47" s="43" t="s">
         <v>6</v>
       </c>
@@ -2601,8 +2601,8 @@
       <c r="R47" s="29"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="85"/>
-      <c r="B48" s="82" t="s">
+      <c r="A48" s="100"/>
+      <c r="B48" s="90" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -2625,8 +2625,8 @@
       <c r="R48" s="60"/>
     </row>
     <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="86"/>
-      <c r="B49" s="88"/>
+      <c r="A49" s="108"/>
+      <c r="B49" s="109"/>
       <c r="C49" s="53" t="s">
         <v>6</v>
       </c>
@@ -2647,8 +2647,8 @@
       <c r="R49" s="48"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="85"/>
-      <c r="B50" s="90" t="s">
+      <c r="A50" s="100"/>
+      <c r="B50" s="110" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="52" t="s">
@@ -2671,8 +2671,8 @@
       <c r="R50" s="51"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="85"/>
-      <c r="B51" s="83"/>
+      <c r="A51" s="100"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="43" t="s">
         <v>6</v>
       </c>
@@ -2693,8 +2693,8 @@
       <c r="R51" s="29"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="85"/>
-      <c r="B52" s="87" t="s">
+      <c r="A52" s="100"/>
+      <c r="B52" s="98" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="54" t="s">
@@ -2717,8 +2717,8 @@
       <c r="R52" s="57"/>
     </row>
     <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="89"/>
-      <c r="B53" s="83"/>
+      <c r="A53" s="102"/>
+      <c r="B53" s="101"/>
       <c r="C53" s="43" t="s">
         <v>6</v>
       </c>
@@ -2733,17 +2733,17 @@
       <c r="L53" s="79"/>
       <c r="M53" s="47"/>
       <c r="N53" s="48"/>
-      <c r="O53" s="48"/>
+      <c r="O53" s="79"/>
       <c r="P53" s="47"/>
       <c r="Q53" s="48"/>
       <c r="R53" s="48"/>
     </row>
     <row r="54" spans="1:18" ht="64.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="91" t="s">
+      <c r="A54" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="92"/>
-      <c r="C54" s="92"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="96"/>
       <c r="D54" s="61" t="s">
         <v>4</v>
       </c>
@@ -2776,14 +2776,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F2"/>
-    <mergeCell ref="G1:I2"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="M1:O2"/>
     <mergeCell ref="B44:B45"/>
@@ -2800,22 +2808,14 @@
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="J1:L2"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F2"/>
+    <mergeCell ref="G1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>